<commit_message>
[ADD]  Map generator, true vision logic.
</commit_message>
<xml_diff>
--- a/_Docs/Tactics.xlsx
+++ b/_Docs/Tactics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
   <si>
     <t>Map Generator</t>
   </si>
@@ -196,6 +196,15 @@
   </si>
   <si>
     <t>View sector,  dark rooms with shorter view distance</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>Jump</t>
+  </si>
+  <si>
+    <t>Over a single tile with height = Half</t>
   </si>
 </sst>
 </file>
@@ -586,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25"/>
@@ -620,6 +629,9 @@
       <c r="B2" s="2" t="s">
         <v>43</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
@@ -627,6 +639,9 @@
       </c>
       <c r="B3" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -740,6 +755,9 @@
       <c r="B22" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="C22" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" s="3" t="s">
@@ -787,7 +805,12 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="3"/>
+      <c r="A29" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="18" thickBot="1">
       <c r="A30" s="4"/>

</xml_diff>

<commit_message>
[ADD]  Proper visibility for units sitting behind half-height objects,  strafe,  proper movement costs.
</commit_message>
<xml_diff>
--- a/_Docs/Tactics.xlsx
+++ b/_Docs/Tactics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
   <si>
     <t>Map Generator</t>
   </si>
@@ -195,9 +195,6 @@
     <t>Obstacles</t>
   </si>
   <si>
-    <t>View sector,  dark rooms with shorter view distance</t>
-  </si>
-  <si>
     <t>v</t>
   </si>
   <si>
@@ -205,6 +202,12 @@
   </si>
   <si>
     <t>Over a single tile with height = Half</t>
+  </si>
+  <si>
+    <t>Dark rooms with shorter view distance</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
@@ -595,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25"/>
@@ -630,7 +633,7 @@
         <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -641,7 +644,7 @@
         <v>44</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -651,6 +654,9 @@
       <c r="B4" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
@@ -658,6 +664,9 @@
       </c>
       <c r="B5" s="2" t="s">
         <v>48</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -756,7 +765,7 @@
         <v>55</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -764,7 +773,7 @@
         <v>16</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -806,10 +815,10 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="18" thickBot="1">

</xml_diff>

<commit_message>
[ADD]  Stairs, Final Target, team generating/locating, proper Item types.
</commit_message>
<xml_diff>
--- a/_Docs/Tactics.xlsx
+++ b/_Docs/Tactics.xlsx
@@ -9,14 +9,14 @@
   <sheets>
     <sheet name="Work Status" sheetId="1" r:id="rId1"/>
     <sheet name="Tables" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Stats" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="79">
   <si>
     <t>Map Generator</t>
   </si>
@@ -208,6 +208,51 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>Time Units</t>
+  </si>
+  <si>
+    <t>Hit Points</t>
+  </si>
+  <si>
+    <t>More time units = more actions per turn,  Restoring to max every turn</t>
+  </si>
+  <si>
+    <t>Slowly restoring (1 per turn),  Less HP = less TU, accuracy and strenght</t>
+  </si>
+  <si>
+    <t>Fire Accuracy</t>
+  </si>
+  <si>
+    <t>Strength</t>
+  </si>
+  <si>
+    <t>Can carry more weight,  better aim with heavy weapons</t>
+  </si>
+  <si>
+    <t>Used for aiming,  can be higher if shoot while sitting</t>
+  </si>
+  <si>
+    <t>maybe can push some terrain objects with good strength?</t>
+  </si>
+  <si>
+    <t>6. Program shooting / aiming / throwing</t>
+  </si>
+  <si>
+    <t>7. Generate monster types.</t>
+  </si>
+  <si>
+    <t>8. Program monsters AI</t>
+  </si>
+  <si>
+    <t>9. Fill levels with appropriate number of monsters</t>
+  </si>
+  <si>
+    <t>TASKS</t>
+  </si>
+  <si>
+    <t>two hands / single hands weapons,  add noise factor</t>
   </si>
 </sst>
 </file>
@@ -282,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -301,6 +346,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -596,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G75"/>
+  <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78:B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25"/>
@@ -783,6 +834,9 @@
       <c r="B24" s="2" t="s">
         <v>58</v>
       </c>
+      <c r="C24" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="3" t="s">
@@ -920,6 +974,9 @@
       <c r="A52" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="B52" s="2" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="2" t="s">
@@ -1015,6 +1072,55 @@
       <c r="A75" s="2" t="s">
         <v>27</v>
       </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="B77" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" s="8"/>
+      <c r="B78" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" s="8"/>
+      <c r="B79" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" s="8"/>
+      <c r="B80" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="8"/>
+      <c r="B81" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="8"/>
+      <c r="B82" s="8"/>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="8"/>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="8"/>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="8"/>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="8"/>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="8"/>
+      <c r="B87" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1038,12 +1144,56 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="100.7109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="53.140625" style="7" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>